<commit_message>
visualização de pedidos quase pronto
</commit_message>
<xml_diff>
--- a/ferias.xlsx
+++ b/ferias.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Sábado</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Atendimento</t>
+  </si>
+  <si>
+    <t>Maria Lima</t>
   </si>
 </sst>
 </file>
@@ -678,7 +681,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -700,6 +703,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1021,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1035,7 +1039,7 @@
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>26</v>
       </c>
@@ -1049,7 +1053,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>31</v>
       </c>
@@ -1063,7 +1067,7 @@
         <v>44817</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>32</v>
       </c>
@@ -1077,7 +1081,7 @@
         <v>44848</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>34</v>
       </c>
@@ -1091,10 +1095,25 @@
         <v>44772</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="9">
+        <v>44743</v>
+      </c>
+      <c r="D5" s="9">
+        <v>44772</v>
+      </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N8" s="6"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I10" s="6"/>
     </row>
   </sheetData>

</xml_diff>